<commit_message>
Add more type annotations
</commit_message>
<xml_diff>
--- a/reports/08-29-19.xlsx
+++ b/reports/08-29-19.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,8 +446,6 @@
           <t>Augusta County</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>7214 Bull Run Post Office Rd, Centreville, 20121</t>
@@ -463,7 +461,56 @@
           <t>0828a867c4</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sumanth  Ratna</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>21:30:59.464162</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>9999</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1A</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ku</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Augusta County</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>7214 Bull Run Post Office Rd, Centreville, 20121</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>a9c7391c8a</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>